<commit_message>
exporting data logic moved the control and util class
</commit_message>
<xml_diff>
--- a/ExportedFiles/excelFiles/monitor_price.xlsx
+++ b/ExportedFiles/excelFiles/monitor_price.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F181"/>
+  <dimension ref="A1:F183"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6225,6 +6225,70 @@
         </is>
       </c>
     </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>2024-10-01 20:15:49</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>monitor_price</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>https://www.bestbuy.com/site/microsoft-xbox-wireless-controller-for-xbox-series-x-xbox-series-s-xbox-one-windows-devices-sky-cipher-special-edition/6584960.p?skuId=6584960</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>$69.99</t>
+        </is>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>2024-10-01</t>
+        </is>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>20:15:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>2024-10-01 20:16:13</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>monitor_price</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>https://www.bestbuy.com/site/microsoft-xbox-wireless-controller-for-xbox-series-x-xbox-series-s-xbox-one-windows-devices-sky-cipher-special-edition/6584960.p?skuId=6584960</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>$69.99</t>
+        </is>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>2024-10-01</t>
+        </is>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>20:16:13</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>